<commit_message>
udpated the template to include extra columns for ligand conc and time step
</commit_message>
<xml_diff>
--- a/submission_example.xlsx
+++ b/submission_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agaspariunas.LIFEARC\projects\studies_endpoint_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F859185-0466-41BF-8BF0-C2455DAC6ED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DB9D39-18CB-4520-98D2-1271430C3030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{350406E5-7FBB-4BED-BF13-A26B7717BB03}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="41">
   <si>
     <t>Object ID</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Test ID</t>
+  </si>
+  <si>
+    <t>ligand_conc</t>
+  </si>
+  <si>
+    <t>time_step</t>
   </si>
 </sst>
 </file>
@@ -528,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65F6FC5-B2FD-4E96-BEEB-B2910050B411}">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,13 +554,14 @@
     <col min="12" max="12" width="15.453125" style="3" customWidth="1"/>
     <col min="13" max="14" width="15.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.90625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="19.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.1796875" style="3"/>
+    <col min="16" max="17" width="17" style="3" customWidth="1"/>
+    <col min="18" max="18" width="32.90625" style="5" customWidth="1"/>
+    <col min="19" max="19" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="19.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -601,19 +608,25 @@
         <v>21</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -653,15 +666,17 @@
       <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="S2" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T2" s="6"/>
+      <c r="U2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -701,15 +716,17 @@
       <c r="O3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R3" s="6"/>
-      <c r="S3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="S3" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T3" s="6"/>
+      <c r="U3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -749,15 +766,17 @@
       <c r="O4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R4" s="6"/>
-      <c r="S4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="S4" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T4" s="6"/>
+      <c r="U4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00177347","02")</f>
         <v>MRT00177347</v>
@@ -798,15 +817,17 @@
       <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R5" s="6"/>
-      <c r="S5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="S5" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T5" s="6"/>
+      <c r="U5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00179688","02")</f>
         <v>MRT00179688</v>
@@ -847,15 +868,17 @@
       <c r="O6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q6" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="S6" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T6" s="6"/>
+      <c r="U6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00150284","02")</f>
         <v>MRT00150284</v>
@@ -896,15 +919,17 @@
       <c r="O7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R7" s="6"/>
-      <c r="S7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="S7" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T7" s="6"/>
+      <c r="U7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00204467","01")</f>
         <v>MRT00204467</v>
@@ -945,15 +970,17 @@
       <c r="O8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q8" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R8" s="6"/>
-      <c r="S8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="S8" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T8" s="6"/>
+      <c r="U8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00125861","02")</f>
         <v>MRT00125861</v>
@@ -994,15 +1021,17 @@
       <c r="O9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R9" s="6"/>
-      <c r="S9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="S9" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T9" s="6"/>
+      <c r="U9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00203968","01")</f>
         <v>MRT00203968</v>
@@ -1043,15 +1072,17 @@
       <c r="O10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R10" s="6"/>
-      <c r="S10" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="S10" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T10" s="6"/>
+      <c r="U10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1091,15 +1122,17 @@
       <c r="O11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q11" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R11" s="6"/>
-      <c r="S11" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="S11" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T11" s="6"/>
+      <c r="U11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1139,15 +1172,17 @@
       <c r="O12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q12" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R12" s="6"/>
-      <c r="S12" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="S12" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T12" s="6"/>
+      <c r="U12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1187,15 +1222,17 @@
       <c r="O13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q13" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R13" s="6"/>
-      <c r="S13" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="S13" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T13" s="6"/>
+      <c r="U13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1235,15 +1272,17 @@
       <c r="O14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q14" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R14" s="6"/>
-      <c r="S14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="S14" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T14" s="6"/>
+      <c r="U14" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1283,15 +1322,17 @@
       <c r="O15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q15" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R15" s="6"/>
-      <c r="S15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="S15" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T15" s="6"/>
+      <c r="U15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00177347","02")</f>
         <v>MRT00177347</v>
@@ -1332,15 +1373,17 @@
       <c r="O16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q16" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R16" s="6"/>
-      <c r="S16" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="S16" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T16" s="6"/>
+      <c r="U16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00179688","02")</f>
         <v>MRT00179688</v>
@@ -1381,15 +1424,17 @@
       <c r="O17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q17" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R17" s="6"/>
-      <c r="S17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="S17" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T17" s="6"/>
+      <c r="U17" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00150284","02")</f>
         <v>MRT00150284</v>
@@ -1430,15 +1475,17 @@
       <c r="O18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q18" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R18" s="6"/>
-      <c r="S18" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="S18" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T18" s="6"/>
+      <c r="U18" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00204467","01")</f>
         <v>MRT00204467</v>
@@ -1479,15 +1526,17 @@
       <c r="O19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q19" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R19" s="6"/>
-      <c r="S19" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="S19" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T19" s="6"/>
+      <c r="U19" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00125861","02")</f>
         <v>MRT00125861</v>
@@ -1528,15 +1577,17 @@
       <c r="O20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q20" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R20" s="6"/>
-      <c r="S20" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="S20" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T20" s="6"/>
+      <c r="U20" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="str">
         <f>CHOOSE(2,"OBJD","MRT00203968","01")</f>
         <v>MRT00203968</v>
@@ -1577,15 +1628,17 @@
       <c r="O21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q21" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R21" s="6"/>
-      <c r="S21" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="S21" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T21" s="6"/>
+      <c r="U21" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1625,15 +1678,17 @@
       <c r="O22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q22" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R22" s="6"/>
-      <c r="S22" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="S22" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T22" s="6"/>
+      <c r="U22" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1673,15 +1728,17 @@
       <c r="O23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q23" s="6">
-        <v>42641</v>
-      </c>
-      <c r="R23" s="6"/>
-      <c r="S23" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="S23" s="6">
+        <v>42641</v>
+      </c>
+      <c r="T23" s="6"/>
+      <c r="U23" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1697,8 +1754,10 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1713,6 +1772,8 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>